<commit_message>
config for .net 5 app release
</commit_message>
<xml_diff>
--- a/mime/application%vnd.openxmlformats-officedocument.spreadsheetml.sheet/test/test.xlsx
+++ b/mime/application%vnd.openxmlformats-officedocument.spreadsheetml.sheet/test/test.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="S1" sheetId="1" r:id="rId1"/>
     <sheet name="S2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.0" hidden="1">'S1'!$B$29</definedName>
@@ -16,7 +17,7 @@
     <definedName name="_xlchart.2" hidden="1">'S1'!$C$29</definedName>
     <definedName name="_xlchart.3" hidden="1">'S1'!$C$30:$C$39</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
   <si>
     <t>T!@#$%^&amp;</t>
   </si>
@@ -48,16 +49,20 @@
   <si>
     <t>AAAAAAAAAAAAAAAAAA</t>
   </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -65,7 +70,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -73,7 +78,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -82,8 +87,15 @@
       <u/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -794,7 +806,7 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" Requires="cx">
+      <mc:Choice xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns="" Requires="cx">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="图表 2"/>
@@ -814,7 +826,7 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvPr id="3" name="矩形 2"/>
             <xdr:cNvSpPr>
               <a:spLocks noTextEdit="1"/>
             </xdr:cNvSpPr>
@@ -1106,7 +1118,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1120,22 +1132,22 @@
       <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.75" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>2</v>
       </c>
@@ -1170,7 +1182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -1184,7 +1196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>2</v>
       </c>
@@ -1192,7 +1204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>1</v>
       </c>
@@ -1200,7 +1212,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>2</v>
       </c>
@@ -1208,7 +1220,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>3</v>
       </c>
@@ -1216,7 +1228,7 @@
         <v>53425</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>4</v>
       </c>
@@ -1224,7 +1236,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>63</v>
       </c>
@@ -1232,7 +1244,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>6</v>
       </c>
@@ -1240,7 +1252,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36">
         <v>7</v>
       </c>
@@ -1248,7 +1260,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37">
         <v>8</v>
       </c>
@@ -1256,7 +1268,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>9</v>
       </c>
@@ -1264,7 +1276,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39">
         <v>20</v>
       </c>
@@ -1273,6 +1285,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B22:L23">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"A"</formula>
@@ -1300,32 +1313,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3333333</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>SUM('S2'!B30:B39)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>